<commit_message>
added collumns for people
</commit_message>
<xml_diff>
--- a/hair-count.xlsx
+++ b/hair-count.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bogdan\Documents\ProjectDataScience\2025-FYP-group10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/mirg_itu_dk/Documents/Dokumenty/ITU/DS_project/2025-FYP-group10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9127D9FF-5CFD-444B-960F-A72E5C20FC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{9127D9FF-5CFD-444B-960F-A72E5C20FC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{680BCA6F-6180-474D-BDD2-E80BD85FDE93}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t>img_1179.png,J</t>
   </si>
@@ -628,16 +628,37 @@
   </si>
   <si>
     <t>File Name</t>
+  </si>
+  <si>
+    <t>Assessment 1 - Mirka</t>
+  </si>
+  <si>
+    <t>Assessment 2 - Bogdan</t>
+  </si>
+  <si>
+    <t>Assessment 4 - Damian</t>
+  </si>
+  <si>
+    <t>Assessment 3 -Asta</t>
+  </si>
+  <si>
+    <t>Assessment 5 - Rudra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -945,1023 +966,1044 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A201"/>
+  <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hair count - Asta
</commit_message>
<xml_diff>
--- a/hair-count.xlsx
+++ b/hair-count.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bogdan\Documents\ProjectDataScience\2025-FYP-group10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astawang/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77EDC45-0210-4A18-A826-4E2522DF2C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AFA0360-47CD-874B-AC77-BB082F2F0E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,6 +671,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -693,8 +699,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,21 +984,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="C202" sqref="C202"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>200</v>
       </c>
@@ -1011,13 +1018,16 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
@@ -1025,13 +1035,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3">
         <v>1</v>
       </c>
@@ -1039,13 +1052,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
       <c r="E4">
         <v>2</v>
       </c>
@@ -1053,13 +1069,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
         <v>0</v>
       </c>
@@ -1067,13 +1086,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6">
         <v>0</v>
       </c>
@@ -1081,13 +1103,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7">
         <v>0</v>
       </c>
@@ -1095,13 +1120,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8">
         <v>1</v>
       </c>
@@ -1109,13 +1137,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
       <c r="E9">
         <v>2</v>
       </c>
@@ -1123,13 +1154,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="E10">
         <v>0</v>
       </c>
@@ -1137,13 +1171,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="E11">
         <v>0</v>
       </c>
@@ -1151,13 +1188,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="E12">
         <v>1</v>
       </c>
@@ -1165,13 +1205,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
       <c r="E13">
         <v>2</v>
       </c>
@@ -1179,13 +1222,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="C14">
         <v>9</v>
       </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
       <c r="E14">
         <v>2</v>
       </c>
@@ -1193,13 +1239,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
       <c r="E15">
         <v>2</v>
       </c>
@@ -1207,13 +1256,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="E16">
         <v>2</v>
       </c>
@@ -1221,13 +1273,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
       <c r="E17">
         <v>2</v>
       </c>
@@ -1235,13 +1290,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
       <c r="E18">
         <v>0</v>
       </c>
@@ -1249,13 +1307,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="C19">
         <v>7</v>
       </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
       <c r="E19">
         <v>2</v>
       </c>
@@ -1263,13 +1324,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
       <c r="E20">
         <v>0</v>
       </c>
@@ -1277,13 +1341,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
       <c r="E21">
         <v>2</v>
       </c>
@@ -1291,13 +1358,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
       <c r="E22">
         <v>1</v>
       </c>
@@ -1305,13 +1375,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
       <c r="E23">
         <v>0</v>
       </c>
@@ -1319,13 +1392,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="C24">
         <v>15</v>
       </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
       <c r="E24">
         <v>2</v>
       </c>
@@ -1333,13 +1409,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
       <c r="E25">
         <v>1</v>
       </c>
@@ -1347,13 +1426,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
       <c r="E26">
         <v>0</v>
       </c>
@@ -1361,13 +1443,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
       <c r="E27">
         <v>2</v>
       </c>
@@ -1375,13 +1460,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="C28">
         <v>5</v>
       </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
       <c r="E28">
         <v>2</v>
       </c>
@@ -1389,13 +1477,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="C29">
         <v>8</v>
       </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
       <c r="E29">
         <v>2</v>
       </c>
@@ -1403,13 +1494,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="C30">
         <v>12</v>
       </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
       <c r="E30">
         <v>2</v>
       </c>
@@ -1417,13 +1511,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
       <c r="E31">
         <v>0</v>
       </c>
@@ -1431,13 +1528,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
       <c r="E32">
         <v>0</v>
       </c>
@@ -1445,13 +1545,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="C33">
         <v>3</v>
       </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
       <c r="E33">
         <v>1</v>
       </c>
@@ -1459,13 +1562,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
       <c r="E34">
         <v>1</v>
       </c>
@@ -1473,13 +1579,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="C35">
         <v>8</v>
       </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
       <c r="E35">
         <v>1</v>
       </c>
@@ -1487,13 +1596,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
       <c r="E36">
         <v>2</v>
       </c>
@@ -1501,13 +1613,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="C37" t="s">
         <v>206</v>
       </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
       <c r="E37">
         <v>1</v>
       </c>
@@ -1515,13 +1630,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
       <c r="E38">
         <v>0</v>
       </c>
@@ -1529,13 +1647,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
       <c r="E39">
         <v>0</v>
       </c>
@@ -1543,13 +1664,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
       <c r="E40">
         <v>0</v>
       </c>
@@ -1557,13 +1681,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
       <c r="E41">
         <v>0</v>
       </c>
@@ -1571,13 +1698,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
       <c r="E42">
         <v>0</v>
       </c>
@@ -1585,13 +1715,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
       <c r="E43">
         <v>0</v>
       </c>
@@ -1599,13 +1732,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="C44">
         <v>6</v>
       </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
       <c r="E44">
         <v>0</v>
       </c>
@@ -1613,13 +1749,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="C45">
         <v>13</v>
       </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
       <c r="E45">
         <v>1</v>
       </c>
@@ -1627,13 +1766,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
       <c r="E46">
         <v>1</v>
       </c>
@@ -1641,13 +1783,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
       <c r="E47">
         <v>0</v>
       </c>
@@ -1655,13 +1800,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
       <c r="E48">
         <v>0</v>
       </c>
@@ -1669,13 +1817,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="C49">
         <v>16</v>
       </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
       <c r="E49">
         <v>1</v>
       </c>
@@ -1683,13 +1834,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
       <c r="E50">
         <v>0</v>
       </c>
@@ -1697,13 +1851,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="C51">
         <v>4</v>
       </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
       <c r="E51">
         <v>1</v>
       </c>
@@ -1711,13 +1868,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="C52">
         <v>11</v>
       </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
       <c r="E52">
         <v>2</v>
       </c>
@@ -1725,13 +1885,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="C53">
         <v>8</v>
       </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
       <c r="E53">
         <v>2</v>
       </c>
@@ -1739,13 +1902,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
       <c r="E54">
         <v>2</v>
       </c>
@@ -1753,13 +1919,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="C55">
         <v>19</v>
       </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
       <c r="E55">
         <v>2</v>
       </c>
@@ -1767,13 +1936,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="C56">
         <v>21</v>
       </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
       <c r="E56">
         <v>1</v>
       </c>
@@ -1781,13 +1953,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
       <c r="E57">
         <v>0</v>
       </c>
@@ -1795,13 +1970,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="C58">
         <v>6</v>
       </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
       <c r="E58">
         <v>1</v>
       </c>
@@ -1809,13 +1987,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
       <c r="E59">
         <v>0</v>
       </c>
@@ -1823,13 +2004,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="C60">
         <v>7</v>
       </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
       <c r="E60">
         <v>1</v>
       </c>
@@ -1837,13 +2021,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
       <c r="E61">
         <v>0</v>
       </c>
@@ -1851,13 +2038,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="C62">
         <v>6</v>
       </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
       <c r="E62">
         <v>1</v>
       </c>
@@ -1865,13 +2055,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="C63">
         <v>3</v>
       </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
       <c r="E63">
         <v>1</v>
       </c>
@@ -1879,13 +2072,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
       <c r="E64">
         <v>0</v>
       </c>
@@ -1893,13 +2089,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="C65">
         <v>3</v>
       </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
       <c r="E65">
         <v>1</v>
       </c>
@@ -1907,13 +2106,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
       <c r="E66">
         <v>0</v>
       </c>
@@ -1921,13 +2123,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
       <c r="E67">
         <v>0</v>
       </c>
@@ -1935,13 +2140,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
       <c r="E68">
         <v>0</v>
       </c>
@@ -1949,13 +2157,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
       <c r="C69">
         <v>7</v>
       </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
       <c r="E69">
         <v>0</v>
       </c>
@@ -1963,13 +2174,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="C70">
         <v>8</v>
       </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
       <c r="E70">
         <v>1</v>
       </c>
@@ -1977,13 +2191,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
       <c r="E71">
         <v>1</v>
       </c>
@@ -1991,13 +2208,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
       <c r="E72">
         <v>1</v>
       </c>
@@ -2005,13 +2225,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
       <c r="E73">
         <v>2</v>
       </c>
@@ -2019,13 +2242,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
       <c r="C74">
         <v>5</v>
       </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
       <c r="E74">
         <v>1</v>
       </c>
@@ -2033,13 +2259,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
       <c r="C75">
         <v>7</v>
       </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
       <c r="E75">
         <v>0</v>
       </c>
@@ -2047,13 +2276,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
       <c r="E76">
         <v>0</v>
       </c>
@@ -2061,13 +2293,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
       <c r="C77">
         <v>9</v>
       </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
       <c r="E77">
         <v>2</v>
       </c>
@@ -2075,13 +2310,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
       <c r="E78">
         <v>0</v>
       </c>
@@ -2089,13 +2327,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
       <c r="C79">
         <v>4</v>
       </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
       <c r="E79">
         <v>1</v>
       </c>
@@ -2103,13 +2344,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
       <c r="C80">
         <v>4</v>
       </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
       <c r="E80">
         <v>2</v>
       </c>
@@ -2117,13 +2361,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
       <c r="E81">
         <v>0</v>
       </c>
@@ -2131,13 +2378,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
       <c r="C82">
         <v>7</v>
       </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
       <c r="E82">
         <v>1</v>
       </c>
@@ -2145,13 +2395,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
       <c r="C83">
         <v>27</v>
       </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
       <c r="E83">
         <v>1</v>
       </c>
@@ -2159,13 +2412,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
       <c r="C84">
         <v>5</v>
       </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
       <c r="E84">
         <v>2</v>
       </c>
@@ -2173,13 +2429,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
       <c r="E85">
         <v>0</v>
       </c>
@@ -2187,13 +2446,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
       <c r="C86">
         <v>11</v>
       </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
       <c r="E86">
         <v>2</v>
       </c>
@@ -2201,13 +2463,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
       <c r="C87">
         <v>8</v>
       </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
       <c r="E87">
         <v>2</v>
       </c>
@@ -2215,13 +2480,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
       <c r="C88">
         <v>0</v>
       </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
       <c r="E88">
         <v>0</v>
       </c>
@@ -2229,13 +2497,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
       <c r="C89">
         <v>4</v>
       </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
       <c r="E89">
         <v>1</v>
       </c>
@@ -2243,13 +2514,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
       <c r="C90">
         <v>5</v>
       </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
       <c r="E90">
         <v>1</v>
       </c>
@@ -2257,13 +2531,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
       <c r="C91">
         <v>0</v>
       </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
       <c r="E91">
         <v>0</v>
       </c>
@@ -2271,13 +2548,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
       <c r="C92">
         <v>9</v>
       </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
       <c r="E92">
         <v>2</v>
       </c>
@@ -2285,13 +2565,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
       <c r="C93">
         <v>0</v>
       </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
       <c r="E93">
         <v>0</v>
       </c>
@@ -2299,13 +2582,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
       <c r="C94">
         <v>5</v>
       </c>
+      <c r="D94">
+        <v>2</v>
+      </c>
       <c r="E94">
         <v>2</v>
       </c>
@@ -2313,13 +2599,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
       <c r="E95">
         <v>1</v>
       </c>
@@ -2327,13 +2616,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
       <c r="E96">
         <v>1</v>
       </c>
@@ -2341,13 +2633,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
       <c r="C97">
         <v>22</v>
       </c>
+      <c r="D97">
+        <v>2</v>
+      </c>
       <c r="E97">
         <v>2</v>
       </c>
@@ -2355,13 +2650,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
       <c r="C98">
         <v>3</v>
       </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
       <c r="E98">
         <v>0</v>
       </c>
@@ -2369,13 +2667,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
       <c r="C99">
         <v>9</v>
       </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
       <c r="E99">
         <v>2</v>
       </c>
@@ -2383,13 +2684,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
       <c r="C100">
         <v>7</v>
       </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
       <c r="E100">
         <v>2</v>
       </c>
@@ -2397,13 +2701,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
       <c r="C101">
         <v>0</v>
       </c>
+      <c r="D101">
+        <v>2</v>
+      </c>
       <c r="E101">
         <v>2</v>
       </c>
@@ -2411,13 +2718,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
       <c r="C102">
         <v>0</v>
       </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
       <c r="E102">
         <v>0</v>
       </c>
@@ -2425,13 +2735,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
       <c r="C103">
         <v>3</v>
       </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
       <c r="E103">
         <v>2</v>
       </c>
@@ -2439,13 +2752,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
       <c r="C104" t="s">
         <v>207</v>
       </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
       <c r="E104">
         <v>2</v>
       </c>
@@ -2453,13 +2769,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
       <c r="C105">
         <v>0</v>
       </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
       <c r="E105">
         <v>0</v>
       </c>
@@ -2467,13 +2786,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
       <c r="C106">
         <v>7</v>
       </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
       <c r="E106">
         <v>2</v>
       </c>
@@ -2481,13 +2803,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
       <c r="C107">
         <v>0</v>
       </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
       <c r="E107">
         <v>0</v>
       </c>
@@ -2495,13 +2820,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
       <c r="C108">
         <v>0</v>
       </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
       <c r="E108">
         <v>0</v>
       </c>
@@ -2509,13 +2837,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
       <c r="C109">
         <v>7</v>
       </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
       <c r="E109">
         <v>0</v>
       </c>
@@ -2523,13 +2854,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
       <c r="C110">
         <v>8</v>
       </c>
+      <c r="D110">
+        <v>2</v>
+      </c>
       <c r="E110">
         <v>1</v>
       </c>
@@ -2537,13 +2871,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
       <c r="C111">
         <v>4</v>
       </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
       <c r="E111">
         <v>2</v>
       </c>
@@ -2551,13 +2888,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
       <c r="C112">
         <v>2</v>
       </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
       <c r="E112">
         <v>2</v>
       </c>
@@ -2565,13 +2905,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
       <c r="C113">
         <v>0</v>
       </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
       <c r="E113">
         <v>0</v>
       </c>
@@ -2579,13 +2922,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
       <c r="C114">
         <v>0</v>
       </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
       <c r="E114">
         <v>2</v>
       </c>
@@ -2593,13 +2939,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
       <c r="C115">
         <v>3</v>
       </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
       <c r="E115">
         <v>1</v>
       </c>
@@ -2607,13 +2956,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
       <c r="C116">
         <v>0</v>
       </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
       <c r="E116">
         <v>0</v>
       </c>
@@ -2621,13 +2973,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
       <c r="C117">
         <v>7</v>
       </c>
+      <c r="D117">
+        <v>2</v>
+      </c>
       <c r="E117">
         <v>2</v>
       </c>
@@ -2635,13 +2990,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
       <c r="C118">
         <v>2</v>
       </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
       <c r="E118">
         <v>1</v>
       </c>
@@ -2649,13 +3007,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
       <c r="C119">
         <v>0</v>
       </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
       <c r="E119">
         <v>0</v>
       </c>
@@ -2663,13 +3024,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
       <c r="C120">
         <v>5</v>
       </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
       <c r="E120">
         <v>2</v>
       </c>
@@ -2677,13 +3041,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
       <c r="C121">
         <v>7</v>
       </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
       <c r="E121">
         <v>0</v>
       </c>
@@ -2691,13 +3058,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
       <c r="C122">
         <v>0</v>
       </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
       <c r="E122">
         <v>0</v>
       </c>
@@ -2705,13 +3075,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
       <c r="C123">
         <v>0</v>
       </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
       <c r="E123">
         <v>0</v>
       </c>
@@ -2719,13 +3092,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
       <c r="C124">
         <v>3</v>
       </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
       <c r="E124">
         <v>1</v>
       </c>
@@ -2733,13 +3109,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
       <c r="C125" t="s">
         <v>208</v>
       </c>
+      <c r="D125">
+        <v>2</v>
+      </c>
       <c r="E125">
         <v>1</v>
       </c>
@@ -2747,13 +3126,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
       <c r="C126">
         <v>0</v>
       </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
       <c r="E126">
         <v>0</v>
       </c>
@@ -2761,13 +3143,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
       <c r="C127">
         <v>5</v>
       </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
       <c r="E127">
         <v>2</v>
       </c>
@@ -2775,13 +3160,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
       <c r="C128">
         <v>7</v>
       </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
       <c r="E128">
         <v>1</v>
       </c>
@@ -2789,13 +3177,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
       <c r="C129">
         <v>0</v>
       </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
       <c r="E129">
         <v>1</v>
       </c>
@@ -2803,13 +3194,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
       <c r="C130">
         <v>0</v>
       </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
       <c r="E130">
         <v>0</v>
       </c>
@@ -2817,13 +3211,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
       <c r="C131">
         <v>0</v>
       </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
       <c r="E131">
         <v>0</v>
       </c>
@@ -2831,13 +3228,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
       <c r="C132">
         <v>0</v>
       </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
       <c r="E132">
         <v>0</v>
       </c>
@@ -2845,13 +3245,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
       <c r="C133">
         <v>4</v>
       </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
       <c r="E133">
         <v>2</v>
       </c>
@@ -2859,13 +3262,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
       <c r="C134">
         <v>3</v>
       </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
       <c r="E134">
         <v>2</v>
       </c>
@@ -2873,13 +3279,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
       <c r="C135">
         <v>4</v>
       </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
       <c r="E135">
         <v>2</v>
       </c>
@@ -2887,13 +3296,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
       <c r="C136">
         <v>7</v>
       </c>
+      <c r="D136">
+        <v>2</v>
+      </c>
       <c r="E136">
         <v>2</v>
       </c>
@@ -2901,13 +3313,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
       <c r="E137">
         <v>0</v>
       </c>
@@ -2915,13 +3330,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
       <c r="C138">
         <v>4</v>
       </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
       <c r="E138">
         <v>2</v>
       </c>
@@ -2929,13 +3347,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
       <c r="C139">
         <v>0</v>
       </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
       <c r="E139">
         <v>0</v>
       </c>
@@ -2943,13 +3364,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
       <c r="C140">
         <v>0</v>
       </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
       <c r="E140">
         <v>0</v>
       </c>
@@ -2957,13 +3381,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
       <c r="C141">
         <v>7</v>
       </c>
+      <c r="D141">
+        <v>2</v>
+      </c>
       <c r="E141">
         <v>2</v>
       </c>
@@ -2971,13 +3398,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
       <c r="C142">
         <v>12</v>
       </c>
+      <c r="D142">
+        <v>2</v>
+      </c>
       <c r="E142">
         <v>2</v>
       </c>
@@ -2985,13 +3415,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
       <c r="C143">
         <v>4</v>
       </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
       <c r="E143">
         <v>1</v>
       </c>
@@ -2999,13 +3432,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>
       <c r="C144">
         <v>0</v>
       </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
       <c r="E144">
         <v>0</v>
       </c>
@@ -3013,13 +3449,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>143</v>
       </c>
       <c r="C145">
         <v>0</v>
       </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
       <c r="E145">
         <v>0</v>
       </c>
@@ -3027,13 +3466,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
       <c r="C146">
         <v>0</v>
       </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
       <c r="E146">
         <v>0</v>
       </c>
@@ -3041,13 +3483,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>145</v>
       </c>
       <c r="C147">
         <v>4</v>
       </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
       <c r="E147">
         <v>0</v>
       </c>
@@ -3055,13 +3500,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>146</v>
       </c>
       <c r="C148">
         <v>0</v>
       </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
       <c r="E148">
         <v>0</v>
       </c>
@@ -3069,13 +3517,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>147</v>
       </c>
       <c r="C149">
         <v>2</v>
       </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
       <c r="E149">
         <v>0</v>
       </c>
@@ -3083,13 +3534,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>148</v>
       </c>
       <c r="C150">
         <v>4</v>
       </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
       <c r="E150">
         <v>0</v>
       </c>
@@ -3097,13 +3551,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>149</v>
       </c>
       <c r="C151">
         <v>0</v>
       </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
       <c r="E151">
         <v>0</v>
       </c>
@@ -3111,13 +3568,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>150</v>
       </c>
       <c r="C152">
         <v>6</v>
       </c>
+      <c r="D152" s="1">
+        <v>2</v>
+      </c>
       <c r="E152">
         <v>0</v>
       </c>
@@ -3125,13 +3585,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
       <c r="C153">
         <v>6</v>
       </c>
+      <c r="D153">
+        <v>2</v>
+      </c>
       <c r="E153">
         <v>1</v>
       </c>
@@ -3139,13 +3602,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>152</v>
       </c>
       <c r="C154">
         <v>0</v>
       </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
       <c r="E154">
         <v>0</v>
       </c>
@@ -3153,13 +3619,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>153</v>
       </c>
       <c r="C155">
         <v>0</v>
       </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
       <c r="E155">
         <v>0</v>
       </c>
@@ -3167,13 +3636,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>154</v>
       </c>
       <c r="C156">
         <v>0</v>
       </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
       <c r="E156">
         <v>0</v>
       </c>
@@ -3181,13 +3653,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>155</v>
       </c>
       <c r="C157">
         <v>0</v>
       </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
       <c r="E157">
         <v>1</v>
       </c>
@@ -3195,13 +3670,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>156</v>
       </c>
       <c r="C158">
         <v>9</v>
       </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
       <c r="E158">
         <v>1</v>
       </c>
@@ -3209,13 +3687,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>157</v>
       </c>
       <c r="C159">
         <v>20</v>
       </c>
+      <c r="D159">
+        <v>2</v>
+      </c>
       <c r="E159">
         <v>2</v>
       </c>
@@ -3223,13 +3704,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>158</v>
       </c>
       <c r="C160">
         <v>0</v>
       </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
       <c r="E160">
         <v>2</v>
       </c>
@@ -3237,13 +3721,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>159</v>
       </c>
       <c r="C161">
         <v>0</v>
       </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
       <c r="E161">
         <v>0</v>
       </c>
@@ -3251,13 +3738,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>160</v>
       </c>
       <c r="C162">
         <v>6</v>
       </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
       <c r="E162">
         <v>1</v>
       </c>
@@ -3265,13 +3755,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>161</v>
       </c>
       <c r="C163">
         <v>11</v>
       </c>
+      <c r="D163">
+        <v>2</v>
+      </c>
       <c r="E163">
         <v>2</v>
       </c>
@@ -3279,13 +3772,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>162</v>
       </c>
       <c r="C164">
         <v>0</v>
       </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
       <c r="E164">
         <v>2</v>
       </c>
@@ -3293,13 +3789,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>163</v>
       </c>
       <c r="C165">
         <v>3</v>
       </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
       <c r="E165">
         <v>0</v>
       </c>
@@ -3307,13 +3806,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>164</v>
       </c>
       <c r="C166">
         <v>5</v>
       </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
       <c r="E166">
         <v>1</v>
       </c>
@@ -3321,13 +3823,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>165</v>
       </c>
       <c r="C167">
         <v>1</v>
       </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
       <c r="E167">
         <v>1</v>
       </c>
@@ -3335,13 +3840,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>166</v>
       </c>
       <c r="C168">
         <v>9</v>
       </c>
+      <c r="D168">
+        <v>2</v>
+      </c>
       <c r="E168">
         <v>1</v>
       </c>
@@ -3349,13 +3857,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>167</v>
       </c>
       <c r="C169">
         <v>6</v>
       </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
       <c r="E169">
         <v>0</v>
       </c>
@@ -3363,13 +3874,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>168</v>
       </c>
       <c r="C170">
         <v>5</v>
       </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
       <c r="E170">
         <v>1</v>
       </c>
@@ -3377,13 +3891,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>169</v>
       </c>
       <c r="C171">
         <v>9</v>
       </c>
+      <c r="D171">
+        <v>2</v>
+      </c>
       <c r="E171">
         <v>1</v>
       </c>
@@ -3391,13 +3908,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>170</v>
       </c>
       <c r="C172">
         <v>6</v>
       </c>
+      <c r="D172">
+        <v>2</v>
+      </c>
       <c r="E172">
         <v>2</v>
       </c>
@@ -3405,13 +3925,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>171</v>
       </c>
       <c r="C173">
         <v>7</v>
       </c>
+      <c r="D173">
+        <v>2</v>
+      </c>
       <c r="E173">
         <v>2</v>
       </c>
@@ -3419,13 +3942,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>172</v>
       </c>
       <c r="C174">
         <v>0</v>
       </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
       <c r="E174">
         <v>2</v>
       </c>
@@ -3433,13 +3959,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>173</v>
       </c>
       <c r="C175">
         <v>0</v>
       </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
       <c r="E175">
         <v>0</v>
       </c>
@@ -3447,13 +3976,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>174</v>
       </c>
       <c r="C176">
         <v>6</v>
       </c>
+      <c r="D176">
+        <v>2</v>
+      </c>
       <c r="E176">
         <v>0</v>
       </c>
@@ -3461,13 +3993,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>175</v>
       </c>
       <c r="C177">
         <v>0</v>
       </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
       <c r="E177">
         <v>1</v>
       </c>
@@ -3475,13 +4010,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>176</v>
       </c>
       <c r="C178">
         <v>1</v>
       </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
       <c r="E178">
         <v>0</v>
       </c>
@@ -3489,13 +4027,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>177</v>
       </c>
       <c r="C179">
         <v>3</v>
       </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
       <c r="E179">
         <v>1</v>
       </c>
@@ -3503,13 +4044,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>178</v>
       </c>
       <c r="C180">
         <v>13</v>
       </c>
+      <c r="D180">
+        <v>2</v>
+      </c>
       <c r="E180">
         <v>2</v>
       </c>
@@ -3517,13 +4061,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>179</v>
       </c>
       <c r="C181">
         <v>0</v>
       </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
       <c r="E181">
         <v>2</v>
       </c>
@@ -3531,13 +4078,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>180</v>
       </c>
       <c r="C182">
         <v>0</v>
       </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
       <c r="E182">
         <v>0</v>
       </c>
@@ -3545,13 +4095,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>181</v>
       </c>
       <c r="C183">
         <v>12</v>
       </c>
+      <c r="D183">
+        <v>2</v>
+      </c>
       <c r="E183">
         <v>0</v>
       </c>
@@ -3559,13 +4112,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>182</v>
       </c>
       <c r="C184">
         <v>0</v>
       </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
       <c r="E184">
         <v>2</v>
       </c>
@@ -3573,13 +4129,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>183</v>
       </c>
       <c r="C185">
         <v>5</v>
       </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
       <c r="E185">
         <v>0</v>
       </c>
@@ -3587,13 +4146,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>184</v>
       </c>
       <c r="C186">
         <v>21</v>
       </c>
+      <c r="D186">
+        <v>2</v>
+      </c>
       <c r="E186">
         <v>0</v>
       </c>
@@ -3601,13 +4163,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>185</v>
       </c>
       <c r="C187">
         <v>12</v>
       </c>
+      <c r="D187">
+        <v>2</v>
+      </c>
       <c r="E187">
         <v>2</v>
       </c>
@@ -3615,13 +4180,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>186</v>
       </c>
       <c r="C188">
         <v>0</v>
       </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
       <c r="E188">
         <v>1</v>
       </c>
@@ -3629,13 +4197,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>187</v>
       </c>
       <c r="C189">
         <v>0</v>
       </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
       <c r="E189">
         <v>0</v>
       </c>
@@ -3643,13 +4214,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>188</v>
       </c>
       <c r="C190">
         <v>0</v>
       </c>
+      <c r="D190">
+        <v>0</v>
+      </c>
       <c r="E190">
         <v>0</v>
       </c>
@@ -3657,13 +4231,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>189</v>
       </c>
       <c r="C191">
         <v>5</v>
       </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
       <c r="E191">
         <v>0</v>
       </c>
@@ -3671,13 +4248,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>190</v>
       </c>
       <c r="C192">
         <v>8</v>
       </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
       <c r="E192">
         <v>0</v>
       </c>
@@ -3685,13 +4265,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>191</v>
       </c>
       <c r="C193">
         <v>5</v>
       </c>
+      <c r="D193">
+        <v>2</v>
+      </c>
       <c r="E193">
         <v>0</v>
       </c>
@@ -3699,13 +4282,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>192</v>
       </c>
       <c r="C194">
         <v>2</v>
       </c>
+      <c r="D194">
+        <v>0</v>
+      </c>
       <c r="E194">
         <v>2</v>
       </c>
@@ -3713,13 +4299,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>193</v>
       </c>
       <c r="C195">
         <v>6</v>
       </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
       <c r="E195">
         <v>0</v>
       </c>
@@ -3727,13 +4316,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>194</v>
       </c>
       <c r="C196">
         <v>0</v>
       </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
       <c r="E196">
         <v>1</v>
       </c>
@@ -3741,13 +4333,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>195</v>
       </c>
       <c r="C197">
         <v>5</v>
       </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
       <c r="E197">
         <v>0</v>
       </c>
@@ -3755,13 +4350,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>196</v>
       </c>
       <c r="C198">
         <v>9</v>
       </c>
+      <c r="D198">
+        <v>2</v>
+      </c>
       <c r="E198">
         <v>0</v>
       </c>
@@ -3769,13 +4367,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>197</v>
       </c>
       <c r="C199">
         <v>12</v>
       </c>
+      <c r="D199">
+        <v>2</v>
+      </c>
       <c r="E199">
         <v>0</v>
       </c>
@@ -3783,13 +4384,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>198</v>
       </c>
       <c r="C200">
         <v>0</v>
       </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
       <c r="E200">
         <v>0</v>
       </c>
@@ -3797,12 +4401,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>199</v>
       </c>
       <c r="C201">
         <v>6</v>
+      </c>
+      <c r="D201">
+        <v>2</v>
       </c>
       <c r="E201">
         <v>0</v>

</xml_diff>

<commit_message>
Added my hair ratings
</commit_message>
<xml_diff>
--- a/hair-count.xlsx
+++ b/hair-count.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astawang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/mirg_itu_dk/Documents/Dokumenty/ITU/DS_project/2025-FYP-group10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AFA0360-47CD-874B-AC77-BB082F2F0E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{6AFA0360-47CD-874B-AC77-BB082F2F0E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B697549-96AA-40A7-BA46-875978C282FA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,6 +717,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -985,20 +989,20 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>200</v>
       </c>
@@ -1018,10 +1022,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="C2">
         <v>0</v>
       </c>
@@ -1035,10 +1042,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3">
         <v>2</v>
       </c>
@@ -1052,8 +1062,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
@@ -1069,10 +1082,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
       <c r="C5">
         <v>0</v>
       </c>
@@ -1086,10 +1102,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
       <c r="C6">
         <v>1</v>
       </c>
@@ -1103,10 +1122,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
       <c r="C7">
         <v>0</v>
       </c>
@@ -1120,10 +1142,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
       <c r="C8">
         <v>3</v>
       </c>
@@ -1137,10 +1162,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
       <c r="C9">
         <v>6</v>
       </c>
@@ -1154,10 +1182,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
       <c r="C10">
         <v>0</v>
       </c>
@@ -1171,10 +1202,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="C11">
         <v>0</v>
       </c>
@@ -1188,10 +1222,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
         <v>4</v>
       </c>
@@ -1205,10 +1242,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
       <c r="C13">
         <v>12</v>
       </c>
@@ -1222,10 +1262,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
       <c r="C14">
         <v>9</v>
       </c>
@@ -1239,10 +1282,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
       <c r="C15">
         <v>0</v>
       </c>
@@ -1256,10 +1302,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>14</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
       <c r="C16">
         <v>6</v>
       </c>
@@ -1273,10 +1322,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
       <c r="C17">
         <v>10</v>
       </c>
@@ -1290,10 +1342,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>16</v>
       </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
       <c r="C18">
         <v>0</v>
       </c>
@@ -1307,10 +1362,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>17</v>
       </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
       <c r="C19">
         <v>7</v>
       </c>
@@ -1324,10 +1382,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>18</v>
       </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
       <c r="C20">
         <v>0</v>
       </c>
@@ -1341,10 +1402,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>19</v>
       </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
       <c r="C21">
         <v>4</v>
       </c>
@@ -1358,10 +1422,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>20</v>
       </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
       <c r="C22">
         <v>4</v>
       </c>
@@ -1375,10 +1442,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>21</v>
       </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
       <c r="C23">
         <v>0</v>
       </c>
@@ -1392,10 +1462,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>22</v>
       </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
       <c r="C24">
         <v>15</v>
       </c>
@@ -1409,10 +1482,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>23</v>
       </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
       <c r="C25">
         <v>4</v>
       </c>
@@ -1426,10 +1502,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>24</v>
       </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
       <c r="C26">
         <v>0</v>
       </c>
@@ -1443,10 +1522,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>25</v>
       </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
       <c r="C27">
         <v>2</v>
       </c>
@@ -1460,10 +1542,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>26</v>
       </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
       <c r="C28">
         <v>5</v>
       </c>
@@ -1477,10 +1562,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>27</v>
       </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
       <c r="C29">
         <v>8</v>
       </c>
@@ -1494,10 +1582,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>28</v>
       </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
       <c r="C30">
         <v>12</v>
       </c>
@@ -1511,10 +1602,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>29</v>
       </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
       <c r="C31">
         <v>0</v>
       </c>
@@ -1528,10 +1622,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>30</v>
       </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
       <c r="C32">
         <v>0</v>
       </c>
@@ -1545,10 +1642,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>31</v>
       </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
       <c r="C33">
         <v>3</v>
       </c>
@@ -1562,10 +1662,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>32</v>
       </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
       <c r="C34">
         <v>4</v>
       </c>
@@ -1579,10 +1682,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>33</v>
       </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
       <c r="C35">
         <v>8</v>
       </c>
@@ -1596,10 +1702,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>34</v>
       </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
       <c r="C36">
         <v>4</v>
       </c>
@@ -1613,10 +1722,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>35</v>
       </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
       <c r="C37" t="s">
         <v>206</v>
       </c>
@@ -1630,10 +1742,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>36</v>
       </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
       <c r="C38">
         <v>0</v>
       </c>
@@ -1647,10 +1762,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>37</v>
       </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
       <c r="C39">
         <v>0</v>
       </c>
@@ -1664,10 +1782,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>38</v>
       </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
       <c r="C40">
         <v>1</v>
       </c>
@@ -1681,10 +1802,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>39</v>
       </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
       <c r="C41">
         <v>0</v>
       </c>
@@ -1698,10 +1822,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>40</v>
       </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
       <c r="C42">
         <v>0</v>
       </c>
@@ -1715,10 +1842,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>41</v>
       </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
       <c r="C43">
         <v>0</v>
       </c>
@@ -1732,10 +1862,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>42</v>
       </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
       <c r="C44">
         <v>6</v>
       </c>
@@ -1749,10 +1882,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>43</v>
       </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
       <c r="C45">
         <v>13</v>
       </c>
@@ -1766,10 +1902,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>44</v>
       </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
       <c r="C46">
         <v>0</v>
       </c>
@@ -1783,10 +1922,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>45</v>
       </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
       <c r="C47">
         <v>0</v>
       </c>
@@ -1800,10 +1942,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>46</v>
       </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
       <c r="C48">
         <v>0</v>
       </c>
@@ -1817,10 +1962,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>47</v>
       </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
       <c r="C49">
         <v>16</v>
       </c>
@@ -1834,10 +1982,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>48</v>
       </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
       <c r="C50">
         <v>0</v>
       </c>
@@ -1851,10 +2002,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>49</v>
       </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
       <c r="C51">
         <v>4</v>
       </c>
@@ -1868,10 +2022,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>50</v>
       </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
       <c r="C52">
         <v>11</v>
       </c>
@@ -1885,10 +2042,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>51</v>
       </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
       <c r="C53">
         <v>8</v>
       </c>
@@ -1902,10 +2062,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>52</v>
       </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
       <c r="C54">
         <v>3</v>
       </c>
@@ -1919,10 +2082,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>53</v>
       </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
       <c r="C55">
         <v>19</v>
       </c>
@@ -1936,10 +2102,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>54</v>
       </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
       <c r="C56">
         <v>21</v>
       </c>
@@ -1953,10 +2122,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>55</v>
       </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
       <c r="C57">
         <v>0</v>
       </c>
@@ -1970,10 +2142,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>56</v>
       </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
       <c r="C58">
         <v>6</v>
       </c>
@@ -1987,10 +2162,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>57</v>
       </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
       <c r="C59">
         <v>0</v>
       </c>
@@ -2004,10 +2182,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>58</v>
       </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
       <c r="C60">
         <v>7</v>
       </c>
@@ -2021,10 +2202,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>59</v>
       </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
       <c r="C61">
         <v>0</v>
       </c>
@@ -2038,10 +2222,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>60</v>
       </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
       <c r="C62">
         <v>6</v>
       </c>
@@ -2055,10 +2242,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>61</v>
       </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
       <c r="C63">
         <v>3</v>
       </c>
@@ -2072,10 +2262,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>62</v>
       </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
       <c r="C64">
         <v>0</v>
       </c>
@@ -2089,10 +2282,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>63</v>
       </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
       <c r="C65">
         <v>3</v>
       </c>
@@ -2106,10 +2302,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>64</v>
       </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
       <c r="C66">
         <v>0</v>
       </c>
@@ -2123,10 +2322,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>65</v>
       </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
       <c r="C67">
         <v>0</v>
       </c>
@@ -2140,10 +2342,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>66</v>
       </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
       <c r="C68">
         <v>0</v>
       </c>
@@ -2157,10 +2362,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>67</v>
       </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
       <c r="C69">
         <v>7</v>
       </c>
@@ -2174,10 +2382,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>68</v>
       </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
       <c r="C70">
         <v>8</v>
       </c>
@@ -2191,10 +2402,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>69</v>
       </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
       <c r="C71">
         <v>0</v>
       </c>
@@ -2208,10 +2422,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>70</v>
       </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
       <c r="C72">
         <v>0</v>
       </c>
@@ -2225,10 +2442,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>71</v>
       </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
       <c r="C73">
         <v>0</v>
       </c>
@@ -2242,10 +2462,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>72</v>
       </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
       <c r="C74">
         <v>5</v>
       </c>
@@ -2259,10 +2482,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>73</v>
       </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
       <c r="C75">
         <v>7</v>
       </c>
@@ -2276,10 +2502,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>74</v>
       </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
       <c r="C76">
         <v>0</v>
       </c>
@@ -2293,10 +2522,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>75</v>
       </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
       <c r="C77">
         <v>9</v>
       </c>
@@ -2310,10 +2542,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>76</v>
       </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
       <c r="C78">
         <v>1</v>
       </c>
@@ -2327,10 +2562,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>77</v>
       </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
       <c r="C79">
         <v>4</v>
       </c>
@@ -2344,10 +2582,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>78</v>
       </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
       <c r="C80">
         <v>4</v>
       </c>
@@ -2361,10 +2602,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>79</v>
       </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
       <c r="C81">
         <v>0</v>
       </c>
@@ -2378,10 +2622,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>80</v>
       </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
       <c r="C82">
         <v>7</v>
       </c>
@@ -2395,10 +2642,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>81</v>
       </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
       <c r="C83">
         <v>27</v>
       </c>
@@ -2412,10 +2662,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>82</v>
       </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
       <c r="C84">
         <v>5</v>
       </c>
@@ -2429,10 +2682,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>83</v>
       </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
       <c r="C85">
         <v>0</v>
       </c>
@@ -2446,10 +2702,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>84</v>
       </c>
+      <c r="B86">
+        <v>2</v>
+      </c>
       <c r="C86">
         <v>11</v>
       </c>
@@ -2463,10 +2722,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>85</v>
       </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
       <c r="C87">
         <v>8</v>
       </c>
@@ -2480,10 +2742,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>86</v>
       </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
       <c r="C88">
         <v>0</v>
       </c>
@@ -2497,10 +2762,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>87</v>
       </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
       <c r="C89">
         <v>4</v>
       </c>
@@ -2514,10 +2782,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>88</v>
       </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
       <c r="C90">
         <v>5</v>
       </c>
@@ -2531,10 +2802,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>89</v>
       </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
       <c r="C91">
         <v>0</v>
       </c>
@@ -2548,10 +2822,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>90</v>
       </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
       <c r="C92">
         <v>9</v>
       </c>
@@ -2565,10 +2842,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>91</v>
       </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
       <c r="C93">
         <v>0</v>
       </c>
@@ -2582,10 +2862,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>92</v>
       </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
       <c r="C94">
         <v>5</v>
       </c>
@@ -2599,10 +2882,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>93</v>
       </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
       <c r="C95">
         <v>0</v>
       </c>
@@ -2616,10 +2902,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>94</v>
       </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
       <c r="C96">
         <v>0</v>
       </c>
@@ -2633,10 +2922,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>95</v>
       </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
       <c r="C97">
         <v>22</v>
       </c>
@@ -2650,10 +2942,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>96</v>
       </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
       <c r="C98">
         <v>3</v>
       </c>
@@ -2667,10 +2962,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>97</v>
       </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
       <c r="C99">
         <v>9</v>
       </c>
@@ -2684,10 +2982,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>98</v>
       </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
       <c r="C100">
         <v>7</v>
       </c>
@@ -2701,10 +3002,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>99</v>
       </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
       <c r="C101">
         <v>0</v>
       </c>
@@ -2718,10 +3022,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>100</v>
       </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
       <c r="C102">
         <v>0</v>
       </c>
@@ -2735,10 +3042,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>101</v>
       </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
       <c r="C103">
         <v>3</v>
       </c>
@@ -2752,10 +3062,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>102</v>
       </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
       <c r="C104" t="s">
         <v>207</v>
       </c>
@@ -2769,10 +3082,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>103</v>
       </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
       <c r="C105">
         <v>0</v>
       </c>
@@ -2786,10 +3102,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>104</v>
       </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
       <c r="C106">
         <v>7</v>
       </c>
@@ -2803,10 +3122,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>105</v>
       </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
       <c r="C107">
         <v>0</v>
       </c>
@@ -2820,10 +3142,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>106</v>
       </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
       <c r="C108">
         <v>0</v>
       </c>
@@ -2837,10 +3162,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>107</v>
       </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
       <c r="C109">
         <v>7</v>
       </c>
@@ -2854,10 +3182,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>108</v>
       </c>
+      <c r="B110">
+        <v>2</v>
+      </c>
       <c r="C110">
         <v>8</v>
       </c>
@@ -2871,10 +3202,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>109</v>
       </c>
+      <c r="B111">
+        <v>2</v>
+      </c>
       <c r="C111">
         <v>4</v>
       </c>
@@ -2888,10 +3222,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>110</v>
       </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
       <c r="C112">
         <v>2</v>
       </c>
@@ -2905,10 +3242,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>111</v>
       </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
       <c r="C113">
         <v>0</v>
       </c>
@@ -2922,10 +3262,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>112</v>
       </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
       <c r="C114">
         <v>0</v>
       </c>
@@ -2939,10 +3282,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>113</v>
       </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
       <c r="C115">
         <v>3</v>
       </c>
@@ -2956,10 +3302,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>114</v>
       </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
       <c r="C116">
         <v>0</v>
       </c>
@@ -2973,10 +3322,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>115</v>
       </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
       <c r="C117">
         <v>7</v>
       </c>
@@ -2990,10 +3342,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>116</v>
       </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
       <c r="C118">
         <v>2</v>
       </c>
@@ -3007,10 +3362,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>117</v>
       </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
       <c r="C119">
         <v>0</v>
       </c>
@@ -3024,10 +3382,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>118</v>
       </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
       <c r="C120">
         <v>5</v>
       </c>
@@ -3041,10 +3402,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>119</v>
       </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
       <c r="C121">
         <v>7</v>
       </c>
@@ -3058,10 +3422,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>120</v>
       </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
       <c r="C122">
         <v>0</v>
       </c>
@@ -3075,10 +3442,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>121</v>
       </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
       <c r="C123">
         <v>0</v>
       </c>
@@ -3092,10 +3462,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>122</v>
       </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
       <c r="C124">
         <v>3</v>
       </c>
@@ -3109,10 +3482,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>123</v>
       </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
       <c r="C125" t="s">
         <v>208</v>
       </c>
@@ -3126,10 +3502,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>124</v>
       </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
       <c r="C126">
         <v>0</v>
       </c>
@@ -3143,10 +3522,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>125</v>
       </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
       <c r="C127">
         <v>5</v>
       </c>
@@ -3160,10 +3542,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>126</v>
       </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
       <c r="C128">
         <v>7</v>
       </c>
@@ -3177,10 +3562,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>127</v>
       </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
       <c r="C129">
         <v>0</v>
       </c>
@@ -3194,10 +3582,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>128</v>
       </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
       <c r="C130">
         <v>0</v>
       </c>
@@ -3211,10 +3602,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>129</v>
       </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
       <c r="C131">
         <v>0</v>
       </c>
@@ -3228,10 +3622,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>130</v>
       </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
       <c r="C132">
         <v>0</v>
       </c>
@@ -3245,10 +3642,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>131</v>
       </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
       <c r="C133">
         <v>4</v>
       </c>
@@ -3262,10 +3662,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>132</v>
       </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
       <c r="C134">
         <v>3</v>
       </c>
@@ -3279,10 +3682,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>133</v>
       </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
       <c r="C135">
         <v>4</v>
       </c>
@@ -3296,10 +3702,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>134</v>
       </c>
+      <c r="B136">
+        <v>2</v>
+      </c>
       <c r="C136">
         <v>7</v>
       </c>
@@ -3313,10 +3722,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>135</v>
       </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
       <c r="C137">
         <v>1</v>
       </c>
@@ -3330,10 +3742,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>136</v>
       </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
       <c r="C138">
         <v>4</v>
       </c>
@@ -3347,10 +3762,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>137</v>
       </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
       <c r="C139">
         <v>0</v>
       </c>
@@ -3364,10 +3782,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>138</v>
       </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
       <c r="C140">
         <v>0</v>
       </c>
@@ -3381,10 +3802,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>139</v>
       </c>
+      <c r="B141">
+        <v>2</v>
+      </c>
       <c r="C141">
         <v>7</v>
       </c>
@@ -3398,10 +3822,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
         <v>140</v>
       </c>
+      <c r="B142">
+        <v>2</v>
+      </c>
       <c r="C142">
         <v>12</v>
       </c>
@@ -3415,10 +3842,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
         <v>141</v>
       </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
       <c r="C143">
         <v>4</v>
       </c>
@@ -3432,10 +3862,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
         <v>142</v>
       </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
       <c r="C144">
         <v>0</v>
       </c>
@@ -3449,10 +3882,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>143</v>
       </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
       <c r="C145">
         <v>0</v>
       </c>
@@ -3466,10 +3902,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>144</v>
       </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
       <c r="C146">
         <v>0</v>
       </c>
@@ -3483,10 +3922,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>145</v>
       </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
       <c r="C147">
         <v>4</v>
       </c>
@@ -3500,10 +3942,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>146</v>
       </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
       <c r="C148">
         <v>0</v>
       </c>
@@ -3517,10 +3962,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>147</v>
       </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
       <c r="C149">
         <v>2</v>
       </c>
@@ -3534,10 +3982,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>148</v>
       </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
       <c r="C150">
         <v>4</v>
       </c>
@@ -3551,10 +4002,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>149</v>
       </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
       <c r="C151">
         <v>0</v>
       </c>
@@ -3568,10 +4022,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>150</v>
       </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
       <c r="C152">
         <v>6</v>
       </c>
@@ -3585,10 +4042,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>151</v>
       </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
       <c r="C153">
         <v>6</v>
       </c>
@@ -3602,10 +4062,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>152</v>
       </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
       <c r="C154">
         <v>0</v>
       </c>
@@ -3619,10 +4082,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>153</v>
       </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
       <c r="C155">
         <v>0</v>
       </c>
@@ -3636,10 +4102,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>154</v>
       </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
       <c r="C156">
         <v>0</v>
       </c>
@@ -3653,10 +4122,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>155</v>
       </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
       <c r="C157">
         <v>0</v>
       </c>
@@ -3670,10 +4142,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
         <v>156</v>
       </c>
+      <c r="B158">
+        <v>2</v>
+      </c>
       <c r="C158">
         <v>9</v>
       </c>
@@ -3687,10 +4162,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>157</v>
       </c>
+      <c r="B159">
+        <v>2</v>
+      </c>
       <c r="C159">
         <v>20</v>
       </c>
@@ -3704,10 +4182,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>158</v>
       </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
       <c r="C160">
         <v>0</v>
       </c>
@@ -3721,10 +4202,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
         <v>159</v>
       </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
       <c r="C161">
         <v>0</v>
       </c>
@@ -3738,10 +4222,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>160</v>
       </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
       <c r="C162">
         <v>6</v>
       </c>
@@ -3755,10 +4242,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>161</v>
       </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
       <c r="C163">
         <v>11</v>
       </c>
@@ -3772,10 +4262,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6">
       <c r="A164" t="s">
         <v>162</v>
       </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
       <c r="C164">
         <v>0</v>
       </c>
@@ -3789,10 +4282,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>163</v>
       </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
       <c r="C165">
         <v>3</v>
       </c>
@@ -3806,10 +4302,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>164</v>
       </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
       <c r="C166">
         <v>5</v>
       </c>
@@ -3823,10 +4322,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6">
       <c r="A167" t="s">
         <v>165</v>
       </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
       <c r="C167">
         <v>1</v>
       </c>
@@ -3840,10 +4342,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6">
       <c r="A168" t="s">
         <v>166</v>
       </c>
+      <c r="B168">
+        <v>2</v>
+      </c>
       <c r="C168">
         <v>9</v>
       </c>
@@ -3857,10 +4362,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
         <v>167</v>
       </c>
+      <c r="B169">
+        <v>2</v>
+      </c>
       <c r="C169">
         <v>6</v>
       </c>
@@ -3874,10 +4382,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>168</v>
       </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
       <c r="C170">
         <v>5</v>
       </c>
@@ -3891,10 +4402,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6">
       <c r="A171" t="s">
         <v>169</v>
       </c>
+      <c r="B171">
+        <v>2</v>
+      </c>
       <c r="C171">
         <v>9</v>
       </c>
@@ -3908,10 +4422,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>170</v>
       </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
       <c r="C172">
         <v>6</v>
       </c>
@@ -3925,10 +4442,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6">
       <c r="A173" t="s">
         <v>171</v>
       </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
       <c r="C173">
         <v>7</v>
       </c>
@@ -3942,10 +4462,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6">
       <c r="A174" t="s">
         <v>172</v>
       </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
       <c r="C174">
         <v>0</v>
       </c>
@@ -3959,10 +4482,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
         <v>173</v>
       </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
       <c r="C175">
         <v>0</v>
       </c>
@@ -3976,10 +4502,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6">
       <c r="A176" t="s">
         <v>174</v>
       </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
       <c r="C176">
         <v>6</v>
       </c>
@@ -3993,10 +4522,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6">
       <c r="A177" t="s">
         <v>175</v>
       </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
       <c r="C177">
         <v>0</v>
       </c>
@@ -4010,10 +4542,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6">
       <c r="A178" t="s">
         <v>176</v>
       </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
       <c r="C178">
         <v>1</v>
       </c>
@@ -4027,10 +4562,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6">
       <c r="A179" t="s">
         <v>177</v>
       </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
       <c r="C179">
         <v>3</v>
       </c>
@@ -4044,10 +4582,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6">
       <c r="A180" t="s">
         <v>178</v>
       </c>
+      <c r="B180">
+        <v>2</v>
+      </c>
       <c r="C180">
         <v>13</v>
       </c>
@@ -4061,10 +4602,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6">
       <c r="A181" t="s">
         <v>179</v>
       </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
       <c r="C181">
         <v>0</v>
       </c>
@@ -4078,10 +4622,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6">
       <c r="A182" t="s">
         <v>180</v>
       </c>
+      <c r="B182">
+        <v>0</v>
+      </c>
       <c r="C182">
         <v>0</v>
       </c>
@@ -4095,10 +4642,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6">
       <c r="A183" t="s">
         <v>181</v>
       </c>
+      <c r="B183">
+        <v>2</v>
+      </c>
       <c r="C183">
         <v>12</v>
       </c>
@@ -4112,10 +4662,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6">
       <c r="A184" t="s">
         <v>182</v>
       </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
       <c r="C184">
         <v>0</v>
       </c>
@@ -4129,10 +4682,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6">
       <c r="A185" t="s">
         <v>183</v>
       </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
       <c r="C185">
         <v>5</v>
       </c>
@@ -4146,10 +4702,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6">
       <c r="A186" t="s">
         <v>184</v>
       </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
       <c r="C186">
         <v>21</v>
       </c>
@@ -4163,10 +4722,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6">
       <c r="A187" t="s">
         <v>185</v>
       </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
       <c r="C187">
         <v>12</v>
       </c>
@@ -4180,10 +4742,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6">
       <c r="A188" t="s">
         <v>186</v>
       </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
       <c r="C188">
         <v>0</v>
       </c>
@@ -4197,10 +4762,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6">
       <c r="A189" t="s">
         <v>187</v>
       </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
       <c r="C189">
         <v>0</v>
       </c>
@@ -4214,10 +4782,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6">
       <c r="A190" t="s">
         <v>188</v>
       </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
       <c r="C190">
         <v>0</v>
       </c>
@@ -4231,10 +4802,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6">
       <c r="A191" t="s">
         <v>189</v>
       </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
       <c r="C191">
         <v>5</v>
       </c>
@@ -4248,10 +4822,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6">
       <c r="A192" t="s">
         <v>190</v>
       </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
       <c r="C192">
         <v>8</v>
       </c>
@@ -4265,10 +4842,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
         <v>191</v>
       </c>
+      <c r="B193">
+        <v>2</v>
+      </c>
       <c r="C193">
         <v>5</v>
       </c>
@@ -4282,10 +4862,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6">
       <c r="A194" t="s">
         <v>192</v>
       </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
       <c r="C194">
         <v>2</v>
       </c>
@@ -4299,10 +4882,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6">
       <c r="A195" t="s">
         <v>193</v>
       </c>
+      <c r="B195">
+        <v>1</v>
+      </c>
       <c r="C195">
         <v>6</v>
       </c>
@@ -4316,10 +4902,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
         <v>194</v>
       </c>
+      <c r="B196">
+        <v>0</v>
+      </c>
       <c r="C196">
         <v>0</v>
       </c>
@@ -4333,10 +4922,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6">
       <c r="A197" t="s">
         <v>195</v>
       </c>
+      <c r="B197">
+        <v>1</v>
+      </c>
       <c r="C197">
         <v>5</v>
       </c>
@@ -4350,10 +4942,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6">
       <c r="A198" t="s">
         <v>196</v>
       </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
       <c r="C198">
         <v>9</v>
       </c>
@@ -4367,10 +4962,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6">
       <c r="A199" t="s">
         <v>197</v>
       </c>
+      <c r="B199">
+        <v>2</v>
+      </c>
       <c r="C199">
         <v>12</v>
       </c>
@@ -4384,10 +4982,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6">
       <c r="A200" t="s">
         <v>198</v>
       </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
       <c r="C200">
         <v>0</v>
       </c>
@@ -4401,9 +5002,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6">
       <c r="A201" t="s">
         <v>199</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
       </c>
       <c r="C201">
         <v>6</v>

</xml_diff>